<commit_message>
added new functional test cases
</commit_message>
<xml_diff>
--- a/data_collection/adjusted/adjusted_evaluation_results.xlsx
+++ b/data_collection/adjusted/adjusted_evaluation_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgoun\conversational_chatbot\data_collection\adjusted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5601D7-905D-45FC-A05D-100BA767545E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC07E5C8-DED9-4B33-8E5C-AC36C9D73C11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832" xr2:uid="{4AE41843-1CFE-4797-91EC-9B324A7F1E7F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832" activeTab="3" xr2:uid="{4AE41843-1CFE-4797-91EC-9B324A7F1E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="aggr_mean" sheetId="1" r:id="rId1"/>
@@ -328,9 +328,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -341,6 +338,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6974,22 +6974,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.9712499999999999</c:v>
+                  <c:v>2.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7362500000000001</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7562499999999999</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9037500000000001</c:v>
+                  <c:v>3.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9437500000000001</c:v>
+                  <c:v>2.21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7249999999999999</c:v>
+                  <c:v>2.0499999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7061,22 +7061,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.9825000000000002</c:v>
+                  <c:v>2.11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8675000000000002</c:v>
+                  <c:v>2.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.82375</c:v>
+                  <c:v>1.94</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9849999999999999</c:v>
+                  <c:v>2.19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.8212499999999996</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8424999999999998</c:v>
+                  <c:v>1.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7148,22 +7148,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.2650000000000006</c:v>
+                  <c:v>5.83</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9675000000000002</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4912499999999991</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2574999999999998</c:v>
+                  <c:v>5.17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.125</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1012499999999994</c:v>
+                  <c:v>7.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7235,22 +7235,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.7887500000000003</c:v>
+                  <c:v>2.19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8037500000000002</c:v>
+                  <c:v>2.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7299999999999998</c:v>
+                  <c:v>2.11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7874999999999999</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.80125</c:v>
+                  <c:v>2.13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8225</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7322,22 +7322,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.1574999999999998</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.105</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0062499999999996</c:v>
+                  <c:v>2.1800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.98</c:v>
+                  <c:v>2.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2487499999999998</c:v>
+                  <c:v>2.62</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0874999999999999</c:v>
+                  <c:v>2.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7778,22 +7778,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.625</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.625</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.5</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.125</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.75</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.5</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7865,22 +7865,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>35.625</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.875</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.625</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.375</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.25</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.25</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7952,22 +7952,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>27.125</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.125</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.25</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.625</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.375</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8039,22 +8039,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>92.375</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105.25</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97.625</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.375</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>97.75</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>104.75</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8126,22 +8126,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>26.875</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.875</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.75</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.375</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.375</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.375</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -28877,7 +28877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BF3446-2568-4949-9380-D7B3CFFC1A0D}">
   <dimension ref="A1:BF65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
@@ -28899,58 +28899,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
       <c r="AH1" s="1"/>
-      <c r="AI1" s="15" t="s">
+      <c r="AI1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
       <c r="AM1" s="1"/>
-      <c r="AN1" s="15" t="s">
+      <c r="AN1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
       <c r="AR1" s="1"/>
-      <c r="AS1" s="15" t="s">
+      <c r="AS1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
+      <c r="AT1" s="19"/>
+      <c r="AU1" s="19"/>
+      <c r="AV1" s="19"/>
       <c r="AW1" s="1"/>
-      <c r="AX1" s="15" t="s">
+      <c r="AX1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
       <c r="BB1" s="1"/>
-      <c r="BC1" s="15" t="s">
+      <c r="BC1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15"/>
+      <c r="BD1" s="19"/>
+      <c r="BE1" s="19"/>
+      <c r="BF1" s="19"/>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -29038,47 +29038,47 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-      <c r="AD3" s="16" t="s">
+      <c r="AD3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="18"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="17"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="16" t="s">
+      <c r="AI3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
-      <c r="AL3" s="18"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="17"/>
       <c r="AM3" s="1"/>
-      <c r="AN3" s="16" t="s">
+      <c r="AN3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AO3" s="17"/>
-      <c r="AP3" s="17"/>
-      <c r="AQ3" s="18"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="17"/>
       <c r="AR3" s="1"/>
-      <c r="AS3" s="16" t="s">
+      <c r="AS3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AT3" s="17"/>
-      <c r="AU3" s="17"/>
-      <c r="AV3" s="18"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="17"/>
       <c r="AW3" s="1"/>
-      <c r="AX3" s="16" t="s">
+      <c r="AX3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AY3" s="17"/>
-      <c r="AZ3" s="17"/>
-      <c r="BA3" s="18"/>
+      <c r="AY3" s="16"/>
+      <c r="AZ3" s="16"/>
+      <c r="BA3" s="17"/>
       <c r="BB3" s="1"/>
-      <c r="BC3" s="16" t="s">
+      <c r="BC3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="BD3" s="17"/>
-      <c r="BE3" s="17"/>
-      <c r="BF3" s="18"/>
+      <c r="BD3" s="16"/>
+      <c r="BE3" s="16"/>
+      <c r="BF3" s="17"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -29680,14 +29680,14 @@
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -29746,47 +29746,47 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
-      <c r="AD11" s="16" t="s">
+      <c r="AD11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="17"/>
-      <c r="AG11" s="18"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="17"/>
       <c r="AH11" s="1"/>
-      <c r="AI11" s="16" t="s">
+      <c r="AI11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
-      <c r="AL11" s="18"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="17"/>
       <c r="AM11" s="1"/>
-      <c r="AN11" s="16" t="s">
+      <c r="AN11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AO11" s="17"/>
-      <c r="AP11" s="17"/>
-      <c r="AQ11" s="18"/>
+      <c r="AO11" s="16"/>
+      <c r="AP11" s="16"/>
+      <c r="AQ11" s="17"/>
       <c r="AR11" s="1"/>
-      <c r="AS11" s="16" t="s">
+      <c r="AS11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AT11" s="17"/>
-      <c r="AU11" s="17"/>
-      <c r="AV11" s="18"/>
+      <c r="AT11" s="16"/>
+      <c r="AU11" s="16"/>
+      <c r="AV11" s="17"/>
       <c r="AW11" s="1"/>
-      <c r="AX11" s="16" t="s">
+      <c r="AX11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AY11" s="17"/>
-      <c r="AZ11" s="17"/>
-      <c r="BA11" s="18"/>
+      <c r="AY11" s="16"/>
+      <c r="AZ11" s="16"/>
+      <c r="BA11" s="17"/>
       <c r="BB11" s="1"/>
-      <c r="BC11" s="16" t="s">
+      <c r="BC11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="BD11" s="17"/>
-      <c r="BE11" s="17"/>
-      <c r="BF11" s="18"/>
+      <c r="BD11" s="16"/>
+      <c r="BE11" s="16"/>
+      <c r="BF11" s="17"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -30449,58 +30449,58 @@
       <c r="BF18" s="1"/>
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
-      <c r="AD19" s="16" t="s">
+      <c r="AD19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AE19" s="17"/>
-      <c r="AF19" s="17"/>
-      <c r="AG19" s="18"/>
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="16"/>
+      <c r="AG19" s="17"/>
       <c r="AH19" s="1"/>
-      <c r="AI19" s="16" t="s">
+      <c r="AI19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="17"/>
-      <c r="AL19" s="18"/>
+      <c r="AJ19" s="16"/>
+      <c r="AK19" s="16"/>
+      <c r="AL19" s="17"/>
       <c r="AM19" s="1"/>
-      <c r="AN19" s="16" t="s">
+      <c r="AN19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AO19" s="17"/>
-      <c r="AP19" s="17"/>
-      <c r="AQ19" s="18"/>
+      <c r="AO19" s="16"/>
+      <c r="AP19" s="16"/>
+      <c r="AQ19" s="17"/>
       <c r="AR19" s="1"/>
-      <c r="AS19" s="16" t="s">
+      <c r="AS19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AT19" s="17"/>
-      <c r="AU19" s="17"/>
-      <c r="AV19" s="18"/>
+      <c r="AT19" s="16"/>
+      <c r="AU19" s="16"/>
+      <c r="AV19" s="17"/>
       <c r="AW19" s="1"/>
-      <c r="AX19" s="16" t="s">
+      <c r="AX19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AY19" s="17"/>
-      <c r="AZ19" s="17"/>
-      <c r="BA19" s="18"/>
+      <c r="AY19" s="16"/>
+      <c r="AZ19" s="16"/>
+      <c r="BA19" s="17"/>
       <c r="BB19" s="1"/>
-      <c r="BC19" s="16" t="s">
+      <c r="BC19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="BD19" s="17"/>
-      <c r="BE19" s="17"/>
-      <c r="BF19" s="18"/>
+      <c r="BD19" s="16"/>
+      <c r="BE19" s="16"/>
+      <c r="BF19" s="17"/>
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -31187,57 +31187,57 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
-      <c r="AD27" s="16" t="s">
+      <c r="AD27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AE27" s="17"/>
-      <c r="AF27" s="17"/>
-      <c r="AG27" s="18"/>
+      <c r="AE27" s="16"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="17"/>
       <c r="AH27" s="1"/>
-      <c r="AI27" s="16" t="s">
+      <c r="AI27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
-      <c r="AL27" s="18"/>
+      <c r="AJ27" s="16"/>
+      <c r="AK27" s="16"/>
+      <c r="AL27" s="17"/>
       <c r="AM27" s="1"/>
-      <c r="AN27" s="16" t="s">
+      <c r="AN27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AO27" s="17"/>
-      <c r="AP27" s="17"/>
-      <c r="AQ27" s="18"/>
+      <c r="AO27" s="16"/>
+      <c r="AP27" s="16"/>
+      <c r="AQ27" s="17"/>
       <c r="AR27" s="1"/>
-      <c r="AS27" s="16" t="s">
+      <c r="AS27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AT27" s="17"/>
-      <c r="AU27" s="17"/>
-      <c r="AV27" s="18"/>
+      <c r="AT27" s="16"/>
+      <c r="AU27" s="16"/>
+      <c r="AV27" s="17"/>
       <c r="AW27" s="1"/>
-      <c r="AX27" s="16" t="s">
+      <c r="AX27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AY27" s="17"/>
-      <c r="AZ27" s="17"/>
-      <c r="BA27" s="18"/>
+      <c r="AY27" s="16"/>
+      <c r="AZ27" s="16"/>
+      <c r="BA27" s="17"/>
       <c r="BB27" s="1"/>
-      <c r="BC27" s="16" t="s">
+      <c r="BC27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="BD27" s="17"/>
-      <c r="BE27" s="17"/>
-      <c r="BF27" s="18"/>
+      <c r="BD27" s="16"/>
+      <c r="BE27" s="16"/>
+      <c r="BF27" s="17"/>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
       <c r="AA28" s="6" t="s">
         <v>11</v>
       </c>
@@ -31922,47 +31922,47 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
-      <c r="AD35" s="16" t="s">
+      <c r="AD35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="17"/>
-      <c r="AG35" s="18"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="17"/>
       <c r="AH35" s="1"/>
-      <c r="AI35" s="16" t="s">
+      <c r="AI35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
-      <c r="AL35" s="18"/>
+      <c r="AJ35" s="16"/>
+      <c r="AK35" s="16"/>
+      <c r="AL35" s="17"/>
       <c r="AM35" s="1"/>
-      <c r="AN35" s="16" t="s">
+      <c r="AN35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AO35" s="17"/>
-      <c r="AP35" s="17"/>
-      <c r="AQ35" s="18"/>
+      <c r="AO35" s="16"/>
+      <c r="AP35" s="16"/>
+      <c r="AQ35" s="17"/>
       <c r="AR35" s="1"/>
-      <c r="AS35" s="16" t="s">
+      <c r="AS35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AT35" s="17"/>
-      <c r="AU35" s="17"/>
-      <c r="AV35" s="18"/>
+      <c r="AT35" s="16"/>
+      <c r="AU35" s="16"/>
+      <c r="AV35" s="17"/>
       <c r="AW35" s="1"/>
-      <c r="AX35" s="16" t="s">
+      <c r="AX35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AY35" s="17"/>
-      <c r="AZ35" s="17"/>
-      <c r="BA35" s="18"/>
+      <c r="AY35" s="16"/>
+      <c r="AZ35" s="16"/>
+      <c r="BA35" s="17"/>
       <c r="BB35" s="1"/>
-      <c r="BC35" s="16" t="s">
+      <c r="BC35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="BD35" s="17"/>
-      <c r="BE35" s="17"/>
-      <c r="BF35" s="18"/>
+      <c r="BD35" s="16"/>
+      <c r="BE35" s="16"/>
+      <c r="BF35" s="17"/>
     </row>
     <row r="36" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AA36" s="6" t="s">
@@ -32493,47 +32493,47 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
-      <c r="AD43" s="16" t="s">
+      <c r="AD43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AE43" s="17"/>
-      <c r="AF43" s="17"/>
-      <c r="AG43" s="18"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="17"/>
       <c r="AH43" s="1"/>
-      <c r="AI43" s="16" t="s">
+      <c r="AI43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
-      <c r="AL43" s="18"/>
+      <c r="AJ43" s="16"/>
+      <c r="AK43" s="16"/>
+      <c r="AL43" s="17"/>
       <c r="AM43" s="1"/>
-      <c r="AN43" s="16" t="s">
+      <c r="AN43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AO43" s="17"/>
-      <c r="AP43" s="17"/>
-      <c r="AQ43" s="18"/>
+      <c r="AO43" s="16"/>
+      <c r="AP43" s="16"/>
+      <c r="AQ43" s="17"/>
       <c r="AR43" s="1"/>
-      <c r="AS43" s="16" t="s">
+      <c r="AS43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AT43" s="17"/>
-      <c r="AU43" s="17"/>
-      <c r="AV43" s="18"/>
+      <c r="AT43" s="16"/>
+      <c r="AU43" s="16"/>
+      <c r="AV43" s="17"/>
       <c r="AW43" s="1"/>
-      <c r="AX43" s="16" t="s">
+      <c r="AX43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AY43" s="17"/>
-      <c r="AZ43" s="17"/>
-      <c r="BA43" s="18"/>
+      <c r="AY43" s="16"/>
+      <c r="AZ43" s="16"/>
+      <c r="BA43" s="17"/>
       <c r="BB43" s="1"/>
-      <c r="BC43" s="16" t="s">
+      <c r="BC43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="BD43" s="17"/>
-      <c r="BE43" s="17"/>
-      <c r="BF43" s="18"/>
+      <c r="BD43" s="16"/>
+      <c r="BE43" s="16"/>
+      <c r="BF43" s="17"/>
     </row>
     <row r="44" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AA44" s="6" t="s">
@@ -33064,47 +33064,47 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
-      <c r="AD51" s="16" t="s">
+      <c r="AD51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AE51" s="17"/>
-      <c r="AF51" s="17"/>
-      <c r="AG51" s="18"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
+      <c r="AG51" s="17"/>
       <c r="AH51" s="1"/>
-      <c r="AI51" s="16" t="s">
+      <c r="AI51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
-      <c r="AL51" s="18"/>
+      <c r="AJ51" s="16"/>
+      <c r="AK51" s="16"/>
+      <c r="AL51" s="17"/>
       <c r="AM51" s="1"/>
-      <c r="AN51" s="16" t="s">
+      <c r="AN51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AO51" s="17"/>
-      <c r="AP51" s="17"/>
-      <c r="AQ51" s="18"/>
+      <c r="AO51" s="16"/>
+      <c r="AP51" s="16"/>
+      <c r="AQ51" s="17"/>
       <c r="AR51" s="1"/>
-      <c r="AS51" s="16" t="s">
+      <c r="AS51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AT51" s="17"/>
-      <c r="AU51" s="17"/>
-      <c r="AV51" s="18"/>
+      <c r="AT51" s="16"/>
+      <c r="AU51" s="16"/>
+      <c r="AV51" s="17"/>
       <c r="AW51" s="1"/>
-      <c r="AX51" s="16" t="s">
+      <c r="AX51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AY51" s="17"/>
-      <c r="AZ51" s="17"/>
-      <c r="BA51" s="18"/>
+      <c r="AY51" s="16"/>
+      <c r="AZ51" s="16"/>
+      <c r="BA51" s="17"/>
       <c r="BB51" s="1"/>
-      <c r="BC51" s="16" t="s">
+      <c r="BC51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="BD51" s="17"/>
-      <c r="BE51" s="17"/>
-      <c r="BF51" s="18"/>
+      <c r="BD51" s="16"/>
+      <c r="BE51" s="16"/>
+      <c r="BF51" s="17"/>
     </row>
     <row r="52" spans="27:58" x14ac:dyDescent="0.3">
       <c r="AA52" s="6" t="s">
@@ -33635,47 +33635,47 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
       <c r="AC59" s="1"/>
-      <c r="AD59" s="16" t="s">
+      <c r="AD59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AE59" s="17"/>
-      <c r="AF59" s="17"/>
-      <c r="AG59" s="18"/>
+      <c r="AE59" s="16"/>
+      <c r="AF59" s="16"/>
+      <c r="AG59" s="17"/>
       <c r="AH59" s="1"/>
-      <c r="AI59" s="16" t="s">
+      <c r="AI59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AJ59" s="17"/>
-      <c r="AK59" s="17"/>
-      <c r="AL59" s="18"/>
+      <c r="AJ59" s="16"/>
+      <c r="AK59" s="16"/>
+      <c r="AL59" s="17"/>
       <c r="AM59" s="1"/>
-      <c r="AN59" s="16" t="s">
+      <c r="AN59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AO59" s="17"/>
-      <c r="AP59" s="17"/>
-      <c r="AQ59" s="18"/>
+      <c r="AO59" s="16"/>
+      <c r="AP59" s="16"/>
+      <c r="AQ59" s="17"/>
       <c r="AR59" s="1"/>
-      <c r="AS59" s="16" t="s">
+      <c r="AS59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AT59" s="17"/>
-      <c r="AU59" s="17"/>
-      <c r="AV59" s="18"/>
+      <c r="AT59" s="16"/>
+      <c r="AU59" s="16"/>
+      <c r="AV59" s="17"/>
       <c r="AW59" s="1"/>
-      <c r="AX59" s="16" t="s">
+      <c r="AX59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AY59" s="17"/>
-      <c r="AZ59" s="17"/>
-      <c r="BA59" s="18"/>
+      <c r="AY59" s="16"/>
+      <c r="AZ59" s="16"/>
+      <c r="BA59" s="17"/>
       <c r="BB59" s="1"/>
-      <c r="BC59" s="16" t="s">
+      <c r="BC59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="BD59" s="17"/>
-      <c r="BE59" s="17"/>
-      <c r="BF59" s="18"/>
+      <c r="BD59" s="16"/>
+      <c r="BE59" s="16"/>
+      <c r="BF59" s="17"/>
     </row>
     <row r="60" spans="27:58" x14ac:dyDescent="0.3">
       <c r="AA60" s="6" t="s">
@@ -34170,36 +34170,19 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="BC59:BF59"/>
-    <mergeCell ref="AD51:AG51"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AN51:AQ51"/>
-    <mergeCell ref="AS51:AV51"/>
-    <mergeCell ref="AX51:BA51"/>
-    <mergeCell ref="BC51:BF51"/>
-    <mergeCell ref="AD59:AG59"/>
-    <mergeCell ref="AI59:AL59"/>
-    <mergeCell ref="AN59:AQ59"/>
-    <mergeCell ref="AS59:AV59"/>
-    <mergeCell ref="AX59:BA59"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="AD35:AG35"/>
-    <mergeCell ref="AI35:AL35"/>
-    <mergeCell ref="AN35:AQ35"/>
-    <mergeCell ref="AS35:AV35"/>
-    <mergeCell ref="BC35:BF35"/>
-    <mergeCell ref="AD43:AG43"/>
-    <mergeCell ref="AI43:AL43"/>
-    <mergeCell ref="AN43:AQ43"/>
-    <mergeCell ref="AS43:AV43"/>
-    <mergeCell ref="AX43:BA43"/>
-    <mergeCell ref="BC43:BF43"/>
-    <mergeCell ref="AX35:BA35"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="AD11:AG11"/>
-    <mergeCell ref="AI11:AL11"/>
-    <mergeCell ref="AN11:AQ11"/>
-    <mergeCell ref="AS11:AV11"/>
+    <mergeCell ref="BC1:BF1"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="AN3:AQ3"/>
+    <mergeCell ref="AS3:AV3"/>
+    <mergeCell ref="AX3:BA3"/>
+    <mergeCell ref="BC3:BF3"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="AS1:AV1"/>
     <mergeCell ref="BC27:BF27"/>
     <mergeCell ref="BC11:BF11"/>
     <mergeCell ref="C19:H19"/>
@@ -34215,19 +34198,36 @@
     <mergeCell ref="AN27:AQ27"/>
     <mergeCell ref="AS27:AV27"/>
     <mergeCell ref="AX27:BA27"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="BC1:BF1"/>
-    <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="AN3:AQ3"/>
-    <mergeCell ref="AS3:AV3"/>
-    <mergeCell ref="AX3:BA3"/>
-    <mergeCell ref="BC3:BF3"/>
-    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="AD11:AG11"/>
+    <mergeCell ref="AI11:AL11"/>
+    <mergeCell ref="AN11:AQ11"/>
+    <mergeCell ref="AS11:AV11"/>
+    <mergeCell ref="BC35:BF35"/>
+    <mergeCell ref="AD43:AG43"/>
+    <mergeCell ref="AI43:AL43"/>
+    <mergeCell ref="AN43:AQ43"/>
+    <mergeCell ref="AS43:AV43"/>
+    <mergeCell ref="AX43:BA43"/>
+    <mergeCell ref="BC43:BF43"/>
+    <mergeCell ref="AX35:BA35"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="AD35:AG35"/>
+    <mergeCell ref="AI35:AL35"/>
+    <mergeCell ref="AN35:AQ35"/>
+    <mergeCell ref="AS35:AV35"/>
+    <mergeCell ref="BC59:BF59"/>
+    <mergeCell ref="AD51:AG51"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AN51:AQ51"/>
+    <mergeCell ref="AS51:AV51"/>
+    <mergeCell ref="AX51:BA51"/>
+    <mergeCell ref="BC51:BF51"/>
+    <mergeCell ref="AD59:AG59"/>
+    <mergeCell ref="AI59:AL59"/>
+    <mergeCell ref="AN59:AQ59"/>
+    <mergeCell ref="AS59:AV59"/>
+    <mergeCell ref="AX59:BA59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -34239,7 +34239,7 @@
   <dimension ref="A1:BF65"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3:BF65"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34260,14 +34260,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
@@ -34399,47 +34399,47 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-      <c r="AD3" s="16" t="s">
+      <c r="AD3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="18"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="17"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="16" t="s">
+      <c r="AI3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
-      <c r="AL3" s="18"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="17"/>
       <c r="AM3" s="1"/>
-      <c r="AN3" s="16" t="s">
+      <c r="AN3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AO3" s="17"/>
-      <c r="AP3" s="17"/>
-      <c r="AQ3" s="18"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="17"/>
       <c r="AR3" s="1"/>
-      <c r="AS3" s="16" t="s">
+      <c r="AS3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AT3" s="17"/>
-      <c r="AU3" s="17"/>
-      <c r="AV3" s="18"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="17"/>
       <c r="AW3" s="1"/>
-      <c r="AX3" s="16" t="s">
+      <c r="AX3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AY3" s="17"/>
-      <c r="AZ3" s="17"/>
-      <c r="BA3" s="18"/>
+      <c r="AY3" s="16"/>
+      <c r="AZ3" s="16"/>
+      <c r="BA3" s="17"/>
       <c r="BB3" s="1"/>
-      <c r="BC3" s="16" t="s">
+      <c r="BC3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="BD3" s="17"/>
-      <c r="BE3" s="17"/>
-      <c r="BF3" s="18"/>
+      <c r="BD3" s="16"/>
+      <c r="BE3" s="16"/>
+      <c r="BF3" s="17"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -35041,14 +35041,14 @@
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -35107,47 +35107,47 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
-      <c r="AD11" s="16" t="s">
+      <c r="AD11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="17"/>
-      <c r="AG11" s="18"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="17"/>
       <c r="AH11" s="1"/>
-      <c r="AI11" s="16" t="s">
+      <c r="AI11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
-      <c r="AL11" s="18"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="17"/>
       <c r="AM11" s="1"/>
-      <c r="AN11" s="16" t="s">
+      <c r="AN11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AO11" s="17"/>
-      <c r="AP11" s="17"/>
-      <c r="AQ11" s="18"/>
+      <c r="AO11" s="16"/>
+      <c r="AP11" s="16"/>
+      <c r="AQ11" s="17"/>
       <c r="AR11" s="1"/>
-      <c r="AS11" s="16" t="s">
+      <c r="AS11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AT11" s="17"/>
-      <c r="AU11" s="17"/>
-      <c r="AV11" s="18"/>
+      <c r="AT11" s="16"/>
+      <c r="AU11" s="16"/>
+      <c r="AV11" s="17"/>
       <c r="AW11" s="1"/>
-      <c r="AX11" s="16" t="s">
+      <c r="AX11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AY11" s="17"/>
-      <c r="AZ11" s="17"/>
-      <c r="BA11" s="18"/>
+      <c r="AY11" s="16"/>
+      <c r="AZ11" s="16"/>
+      <c r="BA11" s="17"/>
       <c r="BB11" s="1"/>
-      <c r="BC11" s="16" t="s">
+      <c r="BC11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="BD11" s="17"/>
-      <c r="BE11" s="17"/>
-      <c r="BF11" s="18"/>
+      <c r="BD11" s="16"/>
+      <c r="BE11" s="16"/>
+      <c r="BF11" s="17"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -35810,58 +35810,58 @@
       <c r="BF18" s="1"/>
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
-      <c r="AD19" s="16" t="s">
+      <c r="AD19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AE19" s="17"/>
-      <c r="AF19" s="17"/>
-      <c r="AG19" s="18"/>
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="16"/>
+      <c r="AG19" s="17"/>
       <c r="AH19" s="1"/>
-      <c r="AI19" s="16" t="s">
+      <c r="AI19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="17"/>
-      <c r="AL19" s="18"/>
+      <c r="AJ19" s="16"/>
+      <c r="AK19" s="16"/>
+      <c r="AL19" s="17"/>
       <c r="AM19" s="1"/>
-      <c r="AN19" s="16" t="s">
+      <c r="AN19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AO19" s="17"/>
-      <c r="AP19" s="17"/>
-      <c r="AQ19" s="18"/>
+      <c r="AO19" s="16"/>
+      <c r="AP19" s="16"/>
+      <c r="AQ19" s="17"/>
       <c r="AR19" s="1"/>
-      <c r="AS19" s="16" t="s">
+      <c r="AS19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AT19" s="17"/>
-      <c r="AU19" s="17"/>
-      <c r="AV19" s="18"/>
+      <c r="AT19" s="16"/>
+      <c r="AU19" s="16"/>
+      <c r="AV19" s="17"/>
       <c r="AW19" s="1"/>
-      <c r="AX19" s="16" t="s">
+      <c r="AX19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AY19" s="17"/>
-      <c r="AZ19" s="17"/>
-      <c r="BA19" s="18"/>
+      <c r="AY19" s="16"/>
+      <c r="AZ19" s="16"/>
+      <c r="BA19" s="17"/>
       <c r="BB19" s="1"/>
-      <c r="BC19" s="16" t="s">
+      <c r="BC19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="BD19" s="17"/>
-      <c r="BE19" s="17"/>
-      <c r="BF19" s="18"/>
+      <c r="BD19" s="16"/>
+      <c r="BE19" s="16"/>
+      <c r="BF19" s="17"/>
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -36548,57 +36548,57 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
-      <c r="AD27" s="16" t="s">
+      <c r="AD27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AE27" s="17"/>
-      <c r="AF27" s="17"/>
-      <c r="AG27" s="18"/>
+      <c r="AE27" s="16"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="17"/>
       <c r="AH27" s="1"/>
-      <c r="AI27" s="16" t="s">
+      <c r="AI27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
-      <c r="AL27" s="18"/>
+      <c r="AJ27" s="16"/>
+      <c r="AK27" s="16"/>
+      <c r="AL27" s="17"/>
       <c r="AM27" s="1"/>
-      <c r="AN27" s="16" t="s">
+      <c r="AN27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AO27" s="17"/>
-      <c r="AP27" s="17"/>
-      <c r="AQ27" s="18"/>
+      <c r="AO27" s="16"/>
+      <c r="AP27" s="16"/>
+      <c r="AQ27" s="17"/>
       <c r="AR27" s="1"/>
-      <c r="AS27" s="16" t="s">
+      <c r="AS27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AT27" s="17"/>
-      <c r="AU27" s="17"/>
-      <c r="AV27" s="18"/>
+      <c r="AT27" s="16"/>
+      <c r="AU27" s="16"/>
+      <c r="AV27" s="17"/>
       <c r="AW27" s="1"/>
-      <c r="AX27" s="16" t="s">
+      <c r="AX27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AY27" s="17"/>
-      <c r="AZ27" s="17"/>
-      <c r="BA27" s="18"/>
+      <c r="AY27" s="16"/>
+      <c r="AZ27" s="16"/>
+      <c r="BA27" s="17"/>
       <c r="BB27" s="1"/>
-      <c r="BC27" s="16" t="s">
+      <c r="BC27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="BD27" s="17"/>
-      <c r="BE27" s="17"/>
-      <c r="BF27" s="18"/>
+      <c r="BD27" s="16"/>
+      <c r="BE27" s="16"/>
+      <c r="BF27" s="17"/>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
       <c r="AA28" s="6" t="s">
         <v>11</v>
       </c>
@@ -37283,47 +37283,47 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
-      <c r="AD35" s="16" t="s">
+      <c r="AD35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="17"/>
-      <c r="AG35" s="18"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="17"/>
       <c r="AH35" s="1"/>
-      <c r="AI35" s="16" t="s">
+      <c r="AI35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
-      <c r="AL35" s="18"/>
+      <c r="AJ35" s="16"/>
+      <c r="AK35" s="16"/>
+      <c r="AL35" s="17"/>
       <c r="AM35" s="1"/>
-      <c r="AN35" s="16" t="s">
+      <c r="AN35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AO35" s="17"/>
-      <c r="AP35" s="17"/>
-      <c r="AQ35" s="18"/>
+      <c r="AO35" s="16"/>
+      <c r="AP35" s="16"/>
+      <c r="AQ35" s="17"/>
       <c r="AR35" s="1"/>
-      <c r="AS35" s="16" t="s">
+      <c r="AS35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AT35" s="17"/>
-      <c r="AU35" s="17"/>
-      <c r="AV35" s="18"/>
+      <c r="AT35" s="16"/>
+      <c r="AU35" s="16"/>
+      <c r="AV35" s="17"/>
       <c r="AW35" s="1"/>
-      <c r="AX35" s="16" t="s">
+      <c r="AX35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AY35" s="17"/>
-      <c r="AZ35" s="17"/>
-      <c r="BA35" s="18"/>
+      <c r="AY35" s="16"/>
+      <c r="AZ35" s="16"/>
+      <c r="BA35" s="17"/>
       <c r="BB35" s="1"/>
-      <c r="BC35" s="16" t="s">
+      <c r="BC35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="BD35" s="17"/>
-      <c r="BE35" s="17"/>
-      <c r="BF35" s="18"/>
+      <c r="BD35" s="16"/>
+      <c r="BE35" s="16"/>
+      <c r="BF35" s="17"/>
     </row>
     <row r="36" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AA36" s="6" t="s">
@@ -37854,47 +37854,47 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
-      <c r="AD43" s="16" t="s">
+      <c r="AD43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AE43" s="17"/>
-      <c r="AF43" s="17"/>
-      <c r="AG43" s="18"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="17"/>
       <c r="AH43" s="1"/>
-      <c r="AI43" s="16" t="s">
+      <c r="AI43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
-      <c r="AL43" s="18"/>
+      <c r="AJ43" s="16"/>
+      <c r="AK43" s="16"/>
+      <c r="AL43" s="17"/>
       <c r="AM43" s="1"/>
-      <c r="AN43" s="16" t="s">
+      <c r="AN43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AO43" s="17"/>
-      <c r="AP43" s="17"/>
-      <c r="AQ43" s="18"/>
+      <c r="AO43" s="16"/>
+      <c r="AP43" s="16"/>
+      <c r="AQ43" s="17"/>
       <c r="AR43" s="1"/>
-      <c r="AS43" s="16" t="s">
+      <c r="AS43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AT43" s="17"/>
-      <c r="AU43" s="17"/>
-      <c r="AV43" s="18"/>
+      <c r="AT43" s="16"/>
+      <c r="AU43" s="16"/>
+      <c r="AV43" s="17"/>
       <c r="AW43" s="1"/>
-      <c r="AX43" s="16" t="s">
+      <c r="AX43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AY43" s="17"/>
-      <c r="AZ43" s="17"/>
-      <c r="BA43" s="18"/>
+      <c r="AY43" s="16"/>
+      <c r="AZ43" s="16"/>
+      <c r="BA43" s="17"/>
       <c r="BB43" s="1"/>
-      <c r="BC43" s="16" t="s">
+      <c r="BC43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="BD43" s="17"/>
-      <c r="BE43" s="17"/>
-      <c r="BF43" s="18"/>
+      <c r="BD43" s="16"/>
+      <c r="BE43" s="16"/>
+      <c r="BF43" s="17"/>
     </row>
     <row r="44" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AA44" s="6" t="s">
@@ -38425,47 +38425,47 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
-      <c r="AD51" s="16" t="s">
+      <c r="AD51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AE51" s="17"/>
-      <c r="AF51" s="17"/>
-      <c r="AG51" s="18"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
+      <c r="AG51" s="17"/>
       <c r="AH51" s="1"/>
-      <c r="AI51" s="16" t="s">
+      <c r="AI51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
-      <c r="AL51" s="18"/>
+      <c r="AJ51" s="16"/>
+      <c r="AK51" s="16"/>
+      <c r="AL51" s="17"/>
       <c r="AM51" s="1"/>
-      <c r="AN51" s="16" t="s">
+      <c r="AN51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AO51" s="17"/>
-      <c r="AP51" s="17"/>
-      <c r="AQ51" s="18"/>
+      <c r="AO51" s="16"/>
+      <c r="AP51" s="16"/>
+      <c r="AQ51" s="17"/>
       <c r="AR51" s="1"/>
-      <c r="AS51" s="16" t="s">
+      <c r="AS51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AT51" s="17"/>
-      <c r="AU51" s="17"/>
-      <c r="AV51" s="18"/>
+      <c r="AT51" s="16"/>
+      <c r="AU51" s="16"/>
+      <c r="AV51" s="17"/>
       <c r="AW51" s="1"/>
-      <c r="AX51" s="16" t="s">
+      <c r="AX51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AY51" s="17"/>
-      <c r="AZ51" s="17"/>
-      <c r="BA51" s="18"/>
+      <c r="AY51" s="16"/>
+      <c r="AZ51" s="16"/>
+      <c r="BA51" s="17"/>
       <c r="BB51" s="1"/>
-      <c r="BC51" s="16" t="s">
+      <c r="BC51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="BD51" s="17"/>
-      <c r="BE51" s="17"/>
-      <c r="BF51" s="18"/>
+      <c r="BD51" s="16"/>
+      <c r="BE51" s="16"/>
+      <c r="BF51" s="17"/>
     </row>
     <row r="52" spans="27:58" x14ac:dyDescent="0.3">
       <c r="AA52" s="6" t="s">
@@ -38996,47 +38996,47 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
       <c r="AC59" s="1"/>
-      <c r="AD59" s="16" t="s">
+      <c r="AD59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AE59" s="17"/>
-      <c r="AF59" s="17"/>
-      <c r="AG59" s="18"/>
+      <c r="AE59" s="16"/>
+      <c r="AF59" s="16"/>
+      <c r="AG59" s="17"/>
       <c r="AH59" s="1"/>
-      <c r="AI59" s="16" t="s">
+      <c r="AI59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AJ59" s="17"/>
-      <c r="AK59" s="17"/>
-      <c r="AL59" s="18"/>
+      <c r="AJ59" s="16"/>
+      <c r="AK59" s="16"/>
+      <c r="AL59" s="17"/>
       <c r="AM59" s="1"/>
-      <c r="AN59" s="16" t="s">
+      <c r="AN59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AO59" s="17"/>
-      <c r="AP59" s="17"/>
-      <c r="AQ59" s="18"/>
+      <c r="AO59" s="16"/>
+      <c r="AP59" s="16"/>
+      <c r="AQ59" s="17"/>
       <c r="AR59" s="1"/>
-      <c r="AS59" s="16" t="s">
+      <c r="AS59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AT59" s="17"/>
-      <c r="AU59" s="17"/>
-      <c r="AV59" s="18"/>
+      <c r="AT59" s="16"/>
+      <c r="AU59" s="16"/>
+      <c r="AV59" s="17"/>
       <c r="AW59" s="1"/>
-      <c r="AX59" s="16" t="s">
+      <c r="AX59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AY59" s="17"/>
-      <c r="AZ59" s="17"/>
-      <c r="BA59" s="18"/>
+      <c r="AY59" s="16"/>
+      <c r="AZ59" s="16"/>
+      <c r="BA59" s="17"/>
       <c r="BB59" s="1"/>
-      <c r="BC59" s="16" t="s">
+      <c r="BC59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="BD59" s="17"/>
-      <c r="BE59" s="17"/>
-      <c r="BF59" s="18"/>
+      <c r="BD59" s="16"/>
+      <c r="BE59" s="16"/>
+      <c r="BF59" s="17"/>
     </row>
     <row r="60" spans="27:58" x14ac:dyDescent="0.3">
       <c r="AA60" s="6" t="s">
@@ -39531,24 +39531,31 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="AD11:AG11"/>
-    <mergeCell ref="AI11:AL11"/>
-    <mergeCell ref="AN11:AQ11"/>
-    <mergeCell ref="AS11:AV11"/>
-    <mergeCell ref="BC1:BF1"/>
-    <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="AN3:AQ3"/>
-    <mergeCell ref="AS3:AV3"/>
-    <mergeCell ref="AX3:BA3"/>
-    <mergeCell ref="BC3:BF3"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="BC59:BF59"/>
+    <mergeCell ref="AD51:AG51"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AN51:AQ51"/>
+    <mergeCell ref="AS51:AV51"/>
+    <mergeCell ref="AX51:BA51"/>
+    <mergeCell ref="BC51:BF51"/>
+    <mergeCell ref="AD59:AG59"/>
+    <mergeCell ref="AI59:AL59"/>
+    <mergeCell ref="AN59:AQ59"/>
+    <mergeCell ref="AS59:AV59"/>
+    <mergeCell ref="AX59:BA59"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="AD35:AG35"/>
+    <mergeCell ref="AI35:AL35"/>
+    <mergeCell ref="AN35:AQ35"/>
+    <mergeCell ref="AS35:AV35"/>
+    <mergeCell ref="BC35:BF35"/>
+    <mergeCell ref="AD43:AG43"/>
+    <mergeCell ref="AI43:AL43"/>
+    <mergeCell ref="AN43:AQ43"/>
+    <mergeCell ref="AS43:AV43"/>
+    <mergeCell ref="AX43:BA43"/>
+    <mergeCell ref="BC43:BF43"/>
+    <mergeCell ref="AX35:BA35"/>
     <mergeCell ref="BC27:BF27"/>
     <mergeCell ref="BC11:BF11"/>
     <mergeCell ref="C19:H19"/>
@@ -39564,31 +39571,24 @@
     <mergeCell ref="AS27:AV27"/>
     <mergeCell ref="AX27:BA27"/>
     <mergeCell ref="AX11:BA11"/>
-    <mergeCell ref="BC35:BF35"/>
-    <mergeCell ref="AD43:AG43"/>
-    <mergeCell ref="AI43:AL43"/>
-    <mergeCell ref="AN43:AQ43"/>
-    <mergeCell ref="AS43:AV43"/>
-    <mergeCell ref="AX43:BA43"/>
-    <mergeCell ref="BC43:BF43"/>
-    <mergeCell ref="AX35:BA35"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="AD35:AG35"/>
-    <mergeCell ref="AI35:AL35"/>
-    <mergeCell ref="AN35:AQ35"/>
-    <mergeCell ref="AS35:AV35"/>
-    <mergeCell ref="BC59:BF59"/>
-    <mergeCell ref="AD51:AG51"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AN51:AQ51"/>
-    <mergeCell ref="AS51:AV51"/>
-    <mergeCell ref="AX51:BA51"/>
-    <mergeCell ref="BC51:BF51"/>
-    <mergeCell ref="AD59:AG59"/>
-    <mergeCell ref="AI59:AL59"/>
-    <mergeCell ref="AN59:AQ59"/>
-    <mergeCell ref="AS59:AV59"/>
-    <mergeCell ref="AX59:BA59"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="BC1:BF1"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="AN3:AQ3"/>
+    <mergeCell ref="AS3:AV3"/>
+    <mergeCell ref="AX3:BA3"/>
+    <mergeCell ref="BC3:BF3"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="AD11:AG11"/>
+    <mergeCell ref="AI11:AL11"/>
+    <mergeCell ref="AN11:AQ11"/>
+    <mergeCell ref="AS11:AV11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -39599,8 +39599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480E4B59-09F6-470E-89F7-39BE76A1FF57}">
   <dimension ref="A1:BF65"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3:BF65"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39621,58 +39621,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
       <c r="AH1" s="1"/>
-      <c r="AI1" s="15" t="s">
+      <c r="AI1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
       <c r="AM1" s="1"/>
-      <c r="AN1" s="15" t="s">
+      <c r="AN1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
       <c r="AR1" s="1"/>
-      <c r="AS1" s="15" t="s">
+      <c r="AS1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
+      <c r="AT1" s="19"/>
+      <c r="AU1" s="19"/>
+      <c r="AV1" s="19"/>
       <c r="AW1" s="1"/>
-      <c r="AX1" s="15" t="s">
+      <c r="AX1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
       <c r="BB1" s="1"/>
-      <c r="BC1" s="15" t="s">
+      <c r="BC1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15"/>
+      <c r="BD1" s="19"/>
+      <c r="BE1" s="19"/>
+      <c r="BF1" s="19"/>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -39760,47 +39760,47 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-      <c r="AD3" s="16" t="s">
+      <c r="AD3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="18"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="17"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="16" t="s">
+      <c r="AI3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
-      <c r="AL3" s="18"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="17"/>
       <c r="AM3" s="1"/>
-      <c r="AN3" s="16" t="s">
+      <c r="AN3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AO3" s="17"/>
-      <c r="AP3" s="17"/>
-      <c r="AQ3" s="18"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="17"/>
       <c r="AR3" s="1"/>
-      <c r="AS3" s="16" t="s">
+      <c r="AS3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AT3" s="17"/>
-      <c r="AU3" s="17"/>
-      <c r="AV3" s="18"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="17"/>
       <c r="AW3" s="1"/>
-      <c r="AX3" s="16" t="s">
+      <c r="AX3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AY3" s="17"/>
-      <c r="AZ3" s="17"/>
-      <c r="BA3" s="18"/>
+      <c r="AY3" s="16"/>
+      <c r="AZ3" s="16"/>
+      <c r="BA3" s="17"/>
       <c r="BB3" s="1"/>
-      <c r="BC3" s="16" t="s">
+      <c r="BC3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="BD3" s="17"/>
-      <c r="BE3" s="17"/>
-      <c r="BF3" s="18"/>
+      <c r="BD3" s="16"/>
+      <c r="BE3" s="16"/>
+      <c r="BF3" s="17"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -40402,14 +40402,14 @@
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -40468,47 +40468,47 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
-      <c r="AD11" s="16" t="s">
+      <c r="AD11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="17"/>
-      <c r="AG11" s="18"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="17"/>
       <c r="AH11" s="1"/>
-      <c r="AI11" s="16" t="s">
+      <c r="AI11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
-      <c r="AL11" s="18"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="17"/>
       <c r="AM11" s="1"/>
-      <c r="AN11" s="16" t="s">
+      <c r="AN11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AO11" s="17"/>
-      <c r="AP11" s="17"/>
-      <c r="AQ11" s="18"/>
+      <c r="AO11" s="16"/>
+      <c r="AP11" s="16"/>
+      <c r="AQ11" s="17"/>
       <c r="AR11" s="1"/>
-      <c r="AS11" s="16" t="s">
+      <c r="AS11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AT11" s="17"/>
-      <c r="AU11" s="17"/>
-      <c r="AV11" s="18"/>
+      <c r="AT11" s="16"/>
+      <c r="AU11" s="16"/>
+      <c r="AV11" s="17"/>
       <c r="AW11" s="1"/>
-      <c r="AX11" s="16" t="s">
+      <c r="AX11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AY11" s="17"/>
-      <c r="AZ11" s="17"/>
-      <c r="BA11" s="18"/>
+      <c r="AY11" s="16"/>
+      <c r="AZ11" s="16"/>
+      <c r="BA11" s="17"/>
       <c r="BB11" s="1"/>
-      <c r="BC11" s="16" t="s">
+      <c r="BC11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="BD11" s="17"/>
-      <c r="BE11" s="17"/>
-      <c r="BF11" s="18"/>
+      <c r="BD11" s="16"/>
+      <c r="BE11" s="16"/>
+      <c r="BF11" s="17"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -41171,58 +41171,58 @@
       <c r="BF18" s="1"/>
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
-      <c r="AD19" s="16" t="s">
+      <c r="AD19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AE19" s="17"/>
-      <c r="AF19" s="17"/>
-      <c r="AG19" s="18"/>
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="16"/>
+      <c r="AG19" s="17"/>
       <c r="AH19" s="1"/>
-      <c r="AI19" s="16" t="s">
+      <c r="AI19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="17"/>
-      <c r="AL19" s="18"/>
+      <c r="AJ19" s="16"/>
+      <c r="AK19" s="16"/>
+      <c r="AL19" s="17"/>
       <c r="AM19" s="1"/>
-      <c r="AN19" s="16" t="s">
+      <c r="AN19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AO19" s="17"/>
-      <c r="AP19" s="17"/>
-      <c r="AQ19" s="18"/>
+      <c r="AO19" s="16"/>
+      <c r="AP19" s="16"/>
+      <c r="AQ19" s="17"/>
       <c r="AR19" s="1"/>
-      <c r="AS19" s="16" t="s">
+      <c r="AS19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AT19" s="17"/>
-      <c r="AU19" s="17"/>
-      <c r="AV19" s="18"/>
+      <c r="AT19" s="16"/>
+      <c r="AU19" s="16"/>
+      <c r="AV19" s="17"/>
       <c r="AW19" s="1"/>
-      <c r="AX19" s="16" t="s">
+      <c r="AX19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AY19" s="17"/>
-      <c r="AZ19" s="17"/>
-      <c r="BA19" s="18"/>
+      <c r="AY19" s="16"/>
+      <c r="AZ19" s="16"/>
+      <c r="BA19" s="17"/>
       <c r="BB19" s="1"/>
-      <c r="BC19" s="16" t="s">
+      <c r="BC19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="BD19" s="17"/>
-      <c r="BE19" s="17"/>
-      <c r="BF19" s="18"/>
+      <c r="BD19" s="16"/>
+      <c r="BE19" s="16"/>
+      <c r="BF19" s="17"/>
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -41909,57 +41909,57 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
-      <c r="AD27" s="16" t="s">
+      <c r="AD27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AE27" s="17"/>
-      <c r="AF27" s="17"/>
-      <c r="AG27" s="18"/>
+      <c r="AE27" s="16"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="17"/>
       <c r="AH27" s="1"/>
-      <c r="AI27" s="16" t="s">
+      <c r="AI27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
-      <c r="AL27" s="18"/>
+      <c r="AJ27" s="16"/>
+      <c r="AK27" s="16"/>
+      <c r="AL27" s="17"/>
       <c r="AM27" s="1"/>
-      <c r="AN27" s="16" t="s">
+      <c r="AN27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AO27" s="17"/>
-      <c r="AP27" s="17"/>
-      <c r="AQ27" s="18"/>
+      <c r="AO27" s="16"/>
+      <c r="AP27" s="16"/>
+      <c r="AQ27" s="17"/>
       <c r="AR27" s="1"/>
-      <c r="AS27" s="16" t="s">
+      <c r="AS27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AT27" s="17"/>
-      <c r="AU27" s="17"/>
-      <c r="AV27" s="18"/>
+      <c r="AT27" s="16"/>
+      <c r="AU27" s="16"/>
+      <c r="AV27" s="17"/>
       <c r="AW27" s="1"/>
-      <c r="AX27" s="16" t="s">
+      <c r="AX27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AY27" s="17"/>
-      <c r="AZ27" s="17"/>
-      <c r="BA27" s="18"/>
+      <c r="AY27" s="16"/>
+      <c r="AZ27" s="16"/>
+      <c r="BA27" s="17"/>
       <c r="BB27" s="1"/>
-      <c r="BC27" s="16" t="s">
+      <c r="BC27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="BD27" s="17"/>
-      <c r="BE27" s="17"/>
-      <c r="BF27" s="18"/>
+      <c r="BD27" s="16"/>
+      <c r="BE27" s="16"/>
+      <c r="BF27" s="17"/>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
       <c r="AA28" s="6" t="s">
         <v>11</v>
       </c>
@@ -42644,47 +42644,47 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
-      <c r="AD35" s="16" t="s">
+      <c r="AD35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="17"/>
-      <c r="AG35" s="18"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="17"/>
       <c r="AH35" s="1"/>
-      <c r="AI35" s="16" t="s">
+      <c r="AI35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
-      <c r="AL35" s="18"/>
+      <c r="AJ35" s="16"/>
+      <c r="AK35" s="16"/>
+      <c r="AL35" s="17"/>
       <c r="AM35" s="1"/>
-      <c r="AN35" s="16" t="s">
+      <c r="AN35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AO35" s="17"/>
-      <c r="AP35" s="17"/>
-      <c r="AQ35" s="18"/>
+      <c r="AO35" s="16"/>
+      <c r="AP35" s="16"/>
+      <c r="AQ35" s="17"/>
       <c r="AR35" s="1"/>
-      <c r="AS35" s="16" t="s">
+      <c r="AS35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AT35" s="17"/>
-      <c r="AU35" s="17"/>
-      <c r="AV35" s="18"/>
+      <c r="AT35" s="16"/>
+      <c r="AU35" s="16"/>
+      <c r="AV35" s="17"/>
       <c r="AW35" s="1"/>
-      <c r="AX35" s="16" t="s">
+      <c r="AX35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AY35" s="17"/>
-      <c r="AZ35" s="17"/>
-      <c r="BA35" s="18"/>
+      <c r="AY35" s="16"/>
+      <c r="AZ35" s="16"/>
+      <c r="BA35" s="17"/>
       <c r="BB35" s="1"/>
-      <c r="BC35" s="16" t="s">
+      <c r="BC35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="BD35" s="17"/>
-      <c r="BE35" s="17"/>
-      <c r="BF35" s="18"/>
+      <c r="BD35" s="16"/>
+      <c r="BE35" s="16"/>
+      <c r="BF35" s="17"/>
     </row>
     <row r="36" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AA36" s="6" t="s">
@@ -43215,47 +43215,47 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
-      <c r="AD43" s="16" t="s">
+      <c r="AD43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AE43" s="17"/>
-      <c r="AF43" s="17"/>
-      <c r="AG43" s="18"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="17"/>
       <c r="AH43" s="1"/>
-      <c r="AI43" s="16" t="s">
+      <c r="AI43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
-      <c r="AL43" s="18"/>
+      <c r="AJ43" s="16"/>
+      <c r="AK43" s="16"/>
+      <c r="AL43" s="17"/>
       <c r="AM43" s="1"/>
-      <c r="AN43" s="16" t="s">
+      <c r="AN43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AO43" s="17"/>
-      <c r="AP43" s="17"/>
-      <c r="AQ43" s="18"/>
+      <c r="AO43" s="16"/>
+      <c r="AP43" s="16"/>
+      <c r="AQ43" s="17"/>
       <c r="AR43" s="1"/>
-      <c r="AS43" s="16" t="s">
+      <c r="AS43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AT43" s="17"/>
-      <c r="AU43" s="17"/>
-      <c r="AV43" s="18"/>
+      <c r="AT43" s="16"/>
+      <c r="AU43" s="16"/>
+      <c r="AV43" s="17"/>
       <c r="AW43" s="1"/>
-      <c r="AX43" s="16" t="s">
+      <c r="AX43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AY43" s="17"/>
-      <c r="AZ43" s="17"/>
-      <c r="BA43" s="18"/>
+      <c r="AY43" s="16"/>
+      <c r="AZ43" s="16"/>
+      <c r="BA43" s="17"/>
       <c r="BB43" s="1"/>
-      <c r="BC43" s="16" t="s">
+      <c r="BC43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="BD43" s="17"/>
-      <c r="BE43" s="17"/>
-      <c r="BF43" s="18"/>
+      <c r="BD43" s="16"/>
+      <c r="BE43" s="16"/>
+      <c r="BF43" s="17"/>
     </row>
     <row r="44" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AA44" s="6" t="s">
@@ -43786,47 +43786,47 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
-      <c r="AD51" s="16" t="s">
+      <c r="AD51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AE51" s="17"/>
-      <c r="AF51" s="17"/>
-      <c r="AG51" s="18"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
+      <c r="AG51" s="17"/>
       <c r="AH51" s="1"/>
-      <c r="AI51" s="16" t="s">
+      <c r="AI51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
-      <c r="AL51" s="18"/>
+      <c r="AJ51" s="16"/>
+      <c r="AK51" s="16"/>
+      <c r="AL51" s="17"/>
       <c r="AM51" s="1"/>
-      <c r="AN51" s="16" t="s">
+      <c r="AN51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AO51" s="17"/>
-      <c r="AP51" s="17"/>
-      <c r="AQ51" s="18"/>
+      <c r="AO51" s="16"/>
+      <c r="AP51" s="16"/>
+      <c r="AQ51" s="17"/>
       <c r="AR51" s="1"/>
-      <c r="AS51" s="16" t="s">
+      <c r="AS51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AT51" s="17"/>
-      <c r="AU51" s="17"/>
-      <c r="AV51" s="18"/>
+      <c r="AT51" s="16"/>
+      <c r="AU51" s="16"/>
+      <c r="AV51" s="17"/>
       <c r="AW51" s="1"/>
-      <c r="AX51" s="16" t="s">
+      <c r="AX51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AY51" s="17"/>
-      <c r="AZ51" s="17"/>
-      <c r="BA51" s="18"/>
+      <c r="AY51" s="16"/>
+      <c r="AZ51" s="16"/>
+      <c r="BA51" s="17"/>
       <c r="BB51" s="1"/>
-      <c r="BC51" s="16" t="s">
+      <c r="BC51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="BD51" s="17"/>
-      <c r="BE51" s="17"/>
-      <c r="BF51" s="18"/>
+      <c r="BD51" s="16"/>
+      <c r="BE51" s="16"/>
+      <c r="BF51" s="17"/>
     </row>
     <row r="52" spans="27:58" x14ac:dyDescent="0.3">
       <c r="AA52" s="6" t="s">
@@ -44357,47 +44357,47 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
       <c r="AC59" s="1"/>
-      <c r="AD59" s="16" t="s">
+      <c r="AD59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AE59" s="17"/>
-      <c r="AF59" s="17"/>
-      <c r="AG59" s="18"/>
+      <c r="AE59" s="16"/>
+      <c r="AF59" s="16"/>
+      <c r="AG59" s="17"/>
       <c r="AH59" s="1"/>
-      <c r="AI59" s="16" t="s">
+      <c r="AI59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AJ59" s="17"/>
-      <c r="AK59" s="17"/>
-      <c r="AL59" s="18"/>
+      <c r="AJ59" s="16"/>
+      <c r="AK59" s="16"/>
+      <c r="AL59" s="17"/>
       <c r="AM59" s="1"/>
-      <c r="AN59" s="16" t="s">
+      <c r="AN59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AO59" s="17"/>
-      <c r="AP59" s="17"/>
-      <c r="AQ59" s="18"/>
+      <c r="AO59" s="16"/>
+      <c r="AP59" s="16"/>
+      <c r="AQ59" s="17"/>
       <c r="AR59" s="1"/>
-      <c r="AS59" s="16" t="s">
+      <c r="AS59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AT59" s="17"/>
-      <c r="AU59" s="17"/>
-      <c r="AV59" s="18"/>
+      <c r="AT59" s="16"/>
+      <c r="AU59" s="16"/>
+      <c r="AV59" s="17"/>
       <c r="AW59" s="1"/>
-      <c r="AX59" s="16" t="s">
+      <c r="AX59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AY59" s="17"/>
-      <c r="AZ59" s="17"/>
-      <c r="BA59" s="18"/>
+      <c r="AY59" s="16"/>
+      <c r="AZ59" s="16"/>
+      <c r="BA59" s="17"/>
       <c r="BB59" s="1"/>
-      <c r="BC59" s="16" t="s">
+      <c r="BC59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="BD59" s="17"/>
-      <c r="BE59" s="17"/>
-      <c r="BF59" s="18"/>
+      <c r="BD59" s="16"/>
+      <c r="BE59" s="16"/>
+      <c r="BF59" s="17"/>
     </row>
     <row r="60" spans="27:58" x14ac:dyDescent="0.3">
       <c r="AA60" s="6" t="s">
@@ -44892,24 +44892,31 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="AD11:AG11"/>
-    <mergeCell ref="AI11:AL11"/>
-    <mergeCell ref="AN11:AQ11"/>
-    <mergeCell ref="AS11:AV11"/>
-    <mergeCell ref="BC1:BF1"/>
-    <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="AN3:AQ3"/>
-    <mergeCell ref="AS3:AV3"/>
-    <mergeCell ref="AX3:BA3"/>
-    <mergeCell ref="BC3:BF3"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="BC59:BF59"/>
+    <mergeCell ref="AD51:AG51"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AN51:AQ51"/>
+    <mergeCell ref="AS51:AV51"/>
+    <mergeCell ref="AX51:BA51"/>
+    <mergeCell ref="BC51:BF51"/>
+    <mergeCell ref="AD59:AG59"/>
+    <mergeCell ref="AI59:AL59"/>
+    <mergeCell ref="AN59:AQ59"/>
+    <mergeCell ref="AS59:AV59"/>
+    <mergeCell ref="AX59:BA59"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="AD35:AG35"/>
+    <mergeCell ref="AI35:AL35"/>
+    <mergeCell ref="AN35:AQ35"/>
+    <mergeCell ref="AS35:AV35"/>
+    <mergeCell ref="BC35:BF35"/>
+    <mergeCell ref="AD43:AG43"/>
+    <mergeCell ref="AI43:AL43"/>
+    <mergeCell ref="AN43:AQ43"/>
+    <mergeCell ref="AS43:AV43"/>
+    <mergeCell ref="AX43:BA43"/>
+    <mergeCell ref="BC43:BF43"/>
+    <mergeCell ref="AX35:BA35"/>
     <mergeCell ref="BC27:BF27"/>
     <mergeCell ref="BC11:BF11"/>
     <mergeCell ref="C19:H19"/>
@@ -44925,31 +44932,24 @@
     <mergeCell ref="AS27:AV27"/>
     <mergeCell ref="AX27:BA27"/>
     <mergeCell ref="AX11:BA11"/>
-    <mergeCell ref="BC35:BF35"/>
-    <mergeCell ref="AD43:AG43"/>
-    <mergeCell ref="AI43:AL43"/>
-    <mergeCell ref="AN43:AQ43"/>
-    <mergeCell ref="AS43:AV43"/>
-    <mergeCell ref="AX43:BA43"/>
-    <mergeCell ref="BC43:BF43"/>
-    <mergeCell ref="AX35:BA35"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="AD35:AG35"/>
-    <mergeCell ref="AI35:AL35"/>
-    <mergeCell ref="AN35:AQ35"/>
-    <mergeCell ref="AS35:AV35"/>
-    <mergeCell ref="BC59:BF59"/>
-    <mergeCell ref="AD51:AG51"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AN51:AQ51"/>
-    <mergeCell ref="AS51:AV51"/>
-    <mergeCell ref="AX51:BA51"/>
-    <mergeCell ref="BC51:BF51"/>
-    <mergeCell ref="AD59:AG59"/>
-    <mergeCell ref="AI59:AL59"/>
-    <mergeCell ref="AN59:AQ59"/>
-    <mergeCell ref="AS59:AV59"/>
-    <mergeCell ref="AX59:BA59"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="BC1:BF1"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="AN3:AQ3"/>
+    <mergeCell ref="AS3:AV3"/>
+    <mergeCell ref="AX3:BA3"/>
+    <mergeCell ref="BC3:BF3"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="AD11:AG11"/>
+    <mergeCell ref="AI11:AL11"/>
+    <mergeCell ref="AN11:AQ11"/>
+    <mergeCell ref="AS11:AV11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -44960,8 +44960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B4B23F-FEA7-4968-84A7-45DCD093976F}">
   <dimension ref="A1:BF65"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3:BF65"/>
+    <sheetView tabSelected="1" topLeftCell="T49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD65" sqref="AD65:AH65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44982,58 +44982,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
       <c r="AH1" s="1"/>
-      <c r="AI1" s="15" t="s">
+      <c r="AI1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="19"/>
       <c r="AM1" s="1"/>
-      <c r="AN1" s="15" t="s">
+      <c r="AN1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
       <c r="AR1" s="1"/>
-      <c r="AS1" s="15" t="s">
+      <c r="AS1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
+      <c r="AT1" s="19"/>
+      <c r="AU1" s="19"/>
+      <c r="AV1" s="19"/>
       <c r="AW1" s="1"/>
-      <c r="AX1" s="15" t="s">
+      <c r="AX1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
       <c r="BB1" s="1"/>
-      <c r="BC1" s="15" t="s">
+      <c r="BC1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15"/>
+      <c r="BD1" s="19"/>
+      <c r="BE1" s="19"/>
+      <c r="BF1" s="19"/>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -45095,101 +45095,101 @@
         <v>8</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C6" si="0">AVERAGE(AD5,AD13,AD21,AD29,AD37,AD45,AD53,AD61)</f>
-        <v>1.9712499999999999</v>
+        <f>MAX(AD5,AD13,AD21,AD29,AD37,AD45,AD53,AD61)</f>
+        <v>2.62</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D6" si="1">AVERAGE(AI5,AI13,AI21,AI29,AI37,AI45,AI53,AI61)</f>
-        <v>1.7362500000000001</v>
+        <f>MAX(AI5,AI13,AI21,AI29,AI37,AI45,AI53,AI61)</f>
+        <v>2</v>
       </c>
       <c r="E3" s="5">
-        <f>AVERAGE(AN5,AN13,AN21,AN29,AN37,AN45,AN53,AN61)</f>
-        <v>1.7562499999999999</v>
+        <f>MAX(AN5,AN13,AN21,AN29,AN37,AN45,AN53,AN61)</f>
+        <v>2.12</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F6" si="2">AVERAGE(AS5,AS13,AS21,AS29,AS37,AS45,AS53,AS61)</f>
-        <v>1.9037500000000001</v>
+        <f>MAX(AS5,AS13,AS21,AS29,AS37,AS45,AS53,AS61)</f>
+        <v>3.06</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G6" si="3">AVERAGE(AX5,AX13,AX21,AX29,AX37,AX45,AX53,AX61)</f>
-        <v>1.9437500000000001</v>
+        <f>MAX(AX5,AX13,AX21,AX29,AX37,AX45,AX53,AX61)</f>
+        <v>2.21</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" ref="H3:H6" si="4">AVERAGE(BC5,BC13,BC21,BC29,BC37,BC45,BC53,BC61)</f>
-        <v>1.7249999999999999</v>
+        <f>MAX(BC5,BC13,BC21,BC29,BC37,BC45,BC53,BC61)</f>
+        <v>2.0499999999999998</v>
       </c>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-      <c r="AD3" s="16" t="s">
+      <c r="AD3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="18"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="17"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="16" t="s">
+      <c r="AI3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
-      <c r="AL3" s="18"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="17"/>
       <c r="AM3" s="1"/>
-      <c r="AN3" s="16" t="s">
+      <c r="AN3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AO3" s="17"/>
-      <c r="AP3" s="17"/>
-      <c r="AQ3" s="18"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="17"/>
       <c r="AR3" s="1"/>
-      <c r="AS3" s="16" t="s">
+      <c r="AS3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AT3" s="17"/>
-      <c r="AU3" s="17"/>
-      <c r="AV3" s="18"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="17"/>
       <c r="AW3" s="1"/>
-      <c r="AX3" s="16" t="s">
+      <c r="AX3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AY3" s="17"/>
-      <c r="AZ3" s="17"/>
-      <c r="BA3" s="18"/>
+      <c r="AY3" s="16"/>
+      <c r="AZ3" s="16"/>
+      <c r="BA3" s="17"/>
       <c r="BB3" s="1"/>
-      <c r="BC3" s="16" t="s">
+      <c r="BC3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="BD3" s="17"/>
-      <c r="BE3" s="17"/>
-      <c r="BF3" s="18"/>
+      <c r="BD3" s="16"/>
+      <c r="BE3" s="16"/>
+      <c r="BF3" s="17"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9825000000000002</v>
+        <f t="shared" ref="C4:C7" si="0">MAX(AD6,AD14,AD22,AD30,AD38,AD46,AD54,AD62)</f>
+        <v>2.11</v>
       </c>
       <c r="D4" s="5">
-        <f t="shared" si="1"/>
-        <v>1.8675000000000002</v>
+        <f t="shared" ref="D4:D7" si="1">MAX(AI6,AI14,AI22,AI30,AI38,AI46,AI54,AI62)</f>
+        <v>2.33</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E7" si="5">AVERAGE(AN6,AN14,AN22,AN30,AN38,AN46,AN54,AN62)</f>
-        <v>1.82375</v>
+        <f t="shared" ref="E4:E7" si="2">MAX(AN6,AN14,AN22,AN30,AN38,AN46,AN54,AN62)</f>
+        <v>1.94</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" si="2"/>
-        <v>1.9849999999999999</v>
+        <f t="shared" ref="F4:F7" si="3">MAX(AS6,AS14,AS22,AS30,AS38,AS46,AS54,AS62)</f>
+        <v>2.19</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" si="3"/>
-        <v>2.8212499999999996</v>
+        <f t="shared" ref="G4:G7" si="4">MAX(AX6,AX14,AX22,AX30,AX38,AX46,AX54,AX62)</f>
+        <v>9</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" si="4"/>
-        <v>1.8424999999999998</v>
+        <f t="shared" ref="H4:H7" si="5">MAX(BC6,BC14,BC22,BC30,BC38,BC46,BC54,BC62)</f>
+        <v>1.95</v>
       </c>
       <c r="AA4" s="6" t="s">
         <v>11</v>
@@ -45282,27 +45282,27 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="0"/>
-        <v>4.2650000000000006</v>
+        <v>5.83</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="1"/>
-        <v>3.9675000000000002</v>
+        <v>5.6</v>
       </c>
       <c r="E5" s="5">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="3"/>
+        <v>5.17</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="4"/>
+        <v>8.4</v>
+      </c>
+      <c r="H5" s="5">
         <f t="shared" si="5"/>
-        <v>4.4912499999999991</v>
-      </c>
-      <c r="F5" s="5">
-        <f t="shared" si="2"/>
-        <v>3.2574999999999998</v>
-      </c>
-      <c r="G5" s="5">
-        <f t="shared" si="3"/>
-        <v>4.125</v>
-      </c>
-      <c r="H5" s="5">
-        <f t="shared" si="4"/>
-        <v>5.1012499999999994</v>
+        <v>7.8</v>
       </c>
       <c r="AA5" s="12" t="s">
         <v>8</v>
@@ -45390,27 +45390,27 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
-        <v>1.7887500000000003</v>
+        <v>2.19</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="1"/>
-        <v>1.8037500000000002</v>
+        <v>2.04</v>
       </c>
       <c r="E6" s="5">
+        <f t="shared" si="2"/>
+        <v>2.11</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="3"/>
+        <v>2.12</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="4"/>
+        <v>2.13</v>
+      </c>
+      <c r="H6" s="5">
         <f t="shared" si="5"/>
-        <v>1.7299999999999998</v>
-      </c>
-      <c r="F6" s="5">
-        <f t="shared" si="2"/>
-        <v>1.7874999999999999</v>
-      </c>
-      <c r="G6" s="5">
-        <f t="shared" si="3"/>
-        <v>1.80125</v>
-      </c>
-      <c r="H6" s="5">
-        <f t="shared" si="4"/>
-        <v>1.8225</v>
+        <v>2.1</v>
       </c>
       <c r="AA6" s="12" t="s">
         <v>10</v>
@@ -45497,28 +45497,28 @@
         <v>19</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(AD9,AD17,AD25,AD33,AD41,AD49,AD57,AD65)</f>
-        <v>2.1574999999999998</v>
+        <f t="shared" si="0"/>
+        <v>2.6</v>
       </c>
       <c r="D7" s="5">
-        <f>AVERAGE(AI9,AI17,AI25,AI33,AI41,AI49,AI57,AI65)</f>
-        <v>2.105</v>
+        <f t="shared" si="1"/>
+        <v>2.6</v>
       </c>
       <c r="E7" s="5">
+        <f t="shared" si="2"/>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="3"/>
+        <v>2.38</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="4"/>
+        <v>2.62</v>
+      </c>
+      <c r="H7" s="5">
         <f t="shared" si="5"/>
-        <v>2.0062499999999996</v>
-      </c>
-      <c r="F7" s="5">
-        <f>AVERAGE(AS9,AS17,AS25,AS33,AS41,AS49,AS57,AS65)</f>
-        <v>1.98</v>
-      </c>
-      <c r="G7" s="5">
-        <f>AVERAGE(AX9,AX17,AX25,AX33,AX41,AX49,AX57,AX65)</f>
-        <v>2.2487499999999998</v>
-      </c>
-      <c r="H7" s="5">
-        <f>AVERAGE(BC9,BC17,BC25,BC33,BC41,BC49,BC57,BC65)</f>
-        <v>2.0874999999999999</v>
+        <v>2.78</v>
       </c>
       <c r="AA7" s="12" t="s">
         <v>17</v>
@@ -45763,14 +45763,14 @@
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -45829,75 +45829,75 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
-      <c r="AD11" s="16" t="s">
+      <c r="AD11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="17"/>
-      <c r="AG11" s="18"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="17"/>
       <c r="AH11" s="1"/>
-      <c r="AI11" s="16" t="s">
+      <c r="AI11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
-      <c r="AL11" s="18"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="17"/>
       <c r="AM11" s="1"/>
-      <c r="AN11" s="16" t="s">
+      <c r="AN11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AO11" s="17"/>
-      <c r="AP11" s="17"/>
-      <c r="AQ11" s="18"/>
+      <c r="AO11" s="16"/>
+      <c r="AP11" s="16"/>
+      <c r="AQ11" s="17"/>
       <c r="AR11" s="1"/>
-      <c r="AS11" s="16" t="s">
+      <c r="AS11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AT11" s="17"/>
-      <c r="AU11" s="17"/>
-      <c r="AV11" s="18"/>
+      <c r="AT11" s="16"/>
+      <c r="AU11" s="16"/>
+      <c r="AV11" s="17"/>
       <c r="AW11" s="1"/>
-      <c r="AX11" s="16" t="s">
+      <c r="AX11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AY11" s="17"/>
-      <c r="AZ11" s="17"/>
-      <c r="BA11" s="18"/>
+      <c r="AY11" s="16"/>
+      <c r="AZ11" s="16"/>
+      <c r="BA11" s="17"/>
       <c r="BB11" s="1"/>
-      <c r="BC11" s="16" t="s">
+      <c r="BC11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="BD11" s="17"/>
-      <c r="BE11" s="17"/>
-      <c r="BF11" s="18"/>
+      <c r="BD11" s="16"/>
+      <c r="BE11" s="16"/>
+      <c r="BF11" s="17"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" ref="C12:C15" si="6">AVERAGE(AE5,AE13,AE21,AE29,AE37,AE45,AE53,AE61)</f>
-        <v>31.625</v>
+        <f>MAX(AE5,AE13,AE21,AE29,AE37,AE45,AE53,AE61)</f>
+        <v>41</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" ref="D12:D15" si="7">AVERAGE(AJ5,AJ13,AJ21,AJ29,AJ37,AJ45,AJ53,AJ61)</f>
-        <v>30.625</v>
+        <f>MAX(AJ5,AJ13,AJ21,AJ29,AJ37,AJ45,AJ53,AJ61)</f>
+        <v>40</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" ref="E12:E15" si="8">AVERAGE(AO5,AO13,AO21,AO29,AO37,AO45,AO53,AO61)</f>
-        <v>32.5</v>
+        <f>MAX(AO5,AO13,AO21,AO29,AO37,AO45,AO53,AO61)</f>
+        <v>43</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" ref="F12:F15" si="9">AVERAGE(AT5,AT13,AT21,AT29,AT37,AT45,AT53,AT61)</f>
-        <v>39.125</v>
+        <f>MAX(AT5,AT13,AT21,AT29,AT37,AT45,AT53,AT61)</f>
+        <v>65</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" ref="G12:G15" si="10">AVERAGE(AY5,AY13,AY21,AY29,AY37,AY45,AY53,AY61)</f>
-        <v>36.75</v>
+        <f>MAX(AY5,AY13,AY21,AY29,AY37,AY45,AY53,AY61)</f>
+        <v>64</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" ref="H12:H15" si="11">AVERAGE(BD5,BD13,BD21,BD29,BD37,BD45,BD53,BD61)</f>
-        <v>34.5</v>
+        <f>MAX(BD5,BD13,BD21,BD29,BD37,BD45,BD53,BD61)</f>
+        <v>49</v>
       </c>
       <c r="AA12" s="6" t="s">
         <v>11</v>
@@ -45989,28 +45989,28 @@
         <v>10</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="6"/>
-        <v>35.625</v>
+        <f t="shared" ref="C13:C16" si="6">MAX(AE6,AE14,AE22,AE30,AE38,AE46,AE54,AE62)</f>
+        <v>38</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="7"/>
-        <v>35.875</v>
+        <f t="shared" ref="D13:D16" si="7">MAX(AJ6,AJ14,AJ22,AJ30,AJ38,AJ46,AJ54,AJ62)</f>
+        <v>42</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="8"/>
-        <v>34.625</v>
+        <f t="shared" ref="E13:E16" si="8">MAX(AO6,AO14,AO22,AO30,AO38,AO46,AO54,AO62)</f>
+        <v>40</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="9"/>
-        <v>36.375</v>
+        <f t="shared" ref="F13:F16" si="9">MAX(AT6,AT14,AT22,AT30,AT38,AT46,AT54,AT62)</f>
+        <v>47</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="10"/>
-        <v>32.25</v>
+        <f t="shared" ref="G13:G16" si="10">MAX(AY6,AY14,AY22,AY30,AY38,AY46,AY54,AY62)</f>
+        <v>37</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="11"/>
-        <v>33.25</v>
+        <f t="shared" ref="H13:H16" si="11">MAX(BD6,BD14,BD22,BD30,BD38,BD46,BD54,BD62)</f>
+        <v>37</v>
       </c>
       <c r="AA13" s="12" t="s">
         <v>8</v>
@@ -46098,27 +46098,27 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" si="6"/>
-        <v>27.125</v>
+        <v>35</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="7"/>
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="8"/>
-        <v>27.125</v>
+        <v>36</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="9"/>
-        <v>19.25</v>
+        <v>31</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="10"/>
-        <v>26.625</v>
+        <v>42</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="11"/>
-        <v>30.375</v>
+        <v>39</v>
       </c>
       <c r="AA14" s="12" t="s">
         <v>10</v>
@@ -46206,27 +46206,27 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" si="6"/>
-        <v>92.375</v>
+        <v>106</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="7"/>
-        <v>105.25</v>
+        <v>125</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="8"/>
-        <v>97.625</v>
+        <v>125</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="9"/>
-        <v>100.375</v>
+        <v>125</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="10"/>
-        <v>97.75</v>
+        <v>119</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="11"/>
-        <v>104.75</v>
+        <v>130</v>
       </c>
       <c r="AA15" s="12" t="s">
         <v>17</v>
@@ -46313,28 +46313,28 @@
         <v>19</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(AE9,AE17,AE25,AE33,AE41,AE49,AE57,AE65)</f>
-        <v>26.875</v>
+        <f t="shared" si="6"/>
+        <v>37</v>
       </c>
       <c r="D16" s="5">
-        <f>AVERAGE(AJ9,AJ17,AJ25,AJ33,AJ41,AJ49,AJ57,AJ65)</f>
-        <v>25.875</v>
+        <f t="shared" si="7"/>
+        <v>30</v>
       </c>
       <c r="E16" s="5">
-        <f>AVERAGE(AO9,AO17,AO25,AO33,AO41,AO49,AO57,AO65)</f>
-        <v>25.75</v>
+        <f t="shared" si="8"/>
+        <v>29</v>
       </c>
       <c r="F16" s="5">
-        <f>AVERAGE(AT9,AT17,AT25,AT33,AT41,AT49,AT57,AT65)</f>
-        <v>25.375</v>
+        <f t="shared" si="9"/>
+        <v>31</v>
       </c>
       <c r="G16" s="5">
-        <f>AVERAGE(AY9,AY17,AY25,AY33,AY41,AY49,AY57,AY65)</f>
-        <v>27.375</v>
+        <f t="shared" si="10"/>
+        <v>42</v>
       </c>
       <c r="H16" s="5">
-        <f>AVERAGE(BD9,BD17,BD25,BD33,BD41,BD49,BD57,BD65)</f>
-        <v>25.375</v>
+        <f t="shared" si="11"/>
+        <v>39</v>
       </c>
       <c r="AA16" s="12" t="s">
         <v>18</v>
@@ -46532,58 +46532,58 @@
       <c r="BF18" s="1"/>
     </row>
     <row r="19" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
-      <c r="AD19" s="16" t="s">
+      <c r="AD19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AE19" s="17"/>
-      <c r="AF19" s="17"/>
-      <c r="AG19" s="18"/>
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="16"/>
+      <c r="AG19" s="17"/>
       <c r="AH19" s="1"/>
-      <c r="AI19" s="16" t="s">
+      <c r="AI19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="17"/>
-      <c r="AL19" s="18"/>
+      <c r="AJ19" s="16"/>
+      <c r="AK19" s="16"/>
+      <c r="AL19" s="17"/>
       <c r="AM19" s="1"/>
-      <c r="AN19" s="16" t="s">
+      <c r="AN19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AO19" s="17"/>
-      <c r="AP19" s="17"/>
-      <c r="AQ19" s="18"/>
+      <c r="AO19" s="16"/>
+      <c r="AP19" s="16"/>
+      <c r="AQ19" s="17"/>
       <c r="AR19" s="1"/>
-      <c r="AS19" s="16" t="s">
+      <c r="AS19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AT19" s="17"/>
-      <c r="AU19" s="17"/>
-      <c r="AV19" s="18"/>
+      <c r="AT19" s="16"/>
+      <c r="AU19" s="16"/>
+      <c r="AV19" s="17"/>
       <c r="AW19" s="1"/>
-      <c r="AX19" s="16" t="s">
+      <c r="AX19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AY19" s="17"/>
-      <c r="AZ19" s="17"/>
-      <c r="BA19" s="18"/>
+      <c r="AY19" s="16"/>
+      <c r="AZ19" s="16"/>
+      <c r="BA19" s="17"/>
       <c r="BB19" s="1"/>
-      <c r="BC19" s="16" t="s">
+      <c r="BC19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="BD19" s="17"/>
-      <c r="BE19" s="17"/>
-      <c r="BF19" s="18"/>
+      <c r="BD19" s="16"/>
+      <c r="BE19" s="16"/>
+      <c r="BF19" s="17"/>
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -47270,57 +47270,57 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
-      <c r="AD27" s="16" t="s">
+      <c r="AD27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AE27" s="17"/>
-      <c r="AF27" s="17"/>
-      <c r="AG27" s="18"/>
+      <c r="AE27" s="16"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="17"/>
       <c r="AH27" s="1"/>
-      <c r="AI27" s="16" t="s">
+      <c r="AI27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
-      <c r="AL27" s="18"/>
+      <c r="AJ27" s="16"/>
+      <c r="AK27" s="16"/>
+      <c r="AL27" s="17"/>
       <c r="AM27" s="1"/>
-      <c r="AN27" s="16" t="s">
+      <c r="AN27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AO27" s="17"/>
-      <c r="AP27" s="17"/>
-      <c r="AQ27" s="18"/>
+      <c r="AO27" s="16"/>
+      <c r="AP27" s="16"/>
+      <c r="AQ27" s="17"/>
       <c r="AR27" s="1"/>
-      <c r="AS27" s="16" t="s">
+      <c r="AS27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AT27" s="17"/>
-      <c r="AU27" s="17"/>
-      <c r="AV27" s="18"/>
+      <c r="AT27" s="16"/>
+      <c r="AU27" s="16"/>
+      <c r="AV27" s="17"/>
       <c r="AW27" s="1"/>
-      <c r="AX27" s="16" t="s">
+      <c r="AX27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AY27" s="17"/>
-      <c r="AZ27" s="17"/>
-      <c r="BA27" s="18"/>
+      <c r="AY27" s="16"/>
+      <c r="AZ27" s="16"/>
+      <c r="BA27" s="17"/>
       <c r="BB27" s="1"/>
-      <c r="BC27" s="16" t="s">
+      <c r="BC27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="BD27" s="17"/>
-      <c r="BE27" s="17"/>
-      <c r="BF27" s="18"/>
+      <c r="BD27" s="16"/>
+      <c r="BE27" s="16"/>
+      <c r="BF27" s="17"/>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
       <c r="AA28" s="6" t="s">
         <v>11</v>
       </c>
@@ -48005,47 +48005,47 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
-      <c r="AD35" s="16" t="s">
+      <c r="AD35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="17"/>
-      <c r="AG35" s="18"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="17"/>
       <c r="AH35" s="1"/>
-      <c r="AI35" s="16" t="s">
+      <c r="AI35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
-      <c r="AL35" s="18"/>
+      <c r="AJ35" s="16"/>
+      <c r="AK35" s="16"/>
+      <c r="AL35" s="17"/>
       <c r="AM35" s="1"/>
-      <c r="AN35" s="16" t="s">
+      <c r="AN35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AO35" s="17"/>
-      <c r="AP35" s="17"/>
-      <c r="AQ35" s="18"/>
+      <c r="AO35" s="16"/>
+      <c r="AP35" s="16"/>
+      <c r="AQ35" s="17"/>
       <c r="AR35" s="1"/>
-      <c r="AS35" s="16" t="s">
+      <c r="AS35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AT35" s="17"/>
-      <c r="AU35" s="17"/>
-      <c r="AV35" s="18"/>
+      <c r="AT35" s="16"/>
+      <c r="AU35" s="16"/>
+      <c r="AV35" s="17"/>
       <c r="AW35" s="1"/>
-      <c r="AX35" s="16" t="s">
+      <c r="AX35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AY35" s="17"/>
-      <c r="AZ35" s="17"/>
-      <c r="BA35" s="18"/>
+      <c r="AY35" s="16"/>
+      <c r="AZ35" s="16"/>
+      <c r="BA35" s="17"/>
       <c r="BB35" s="1"/>
-      <c r="BC35" s="16" t="s">
+      <c r="BC35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="BD35" s="17"/>
-      <c r="BE35" s="17"/>
-      <c r="BF35" s="18"/>
+      <c r="BD35" s="16"/>
+      <c r="BE35" s="16"/>
+      <c r="BF35" s="17"/>
     </row>
     <row r="36" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AA36" s="6" t="s">
@@ -48576,47 +48576,47 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
-      <c r="AD43" s="16" t="s">
+      <c r="AD43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AE43" s="17"/>
-      <c r="AF43" s="17"/>
-      <c r="AG43" s="18"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="17"/>
       <c r="AH43" s="1"/>
-      <c r="AI43" s="16" t="s">
+      <c r="AI43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
-      <c r="AL43" s="18"/>
+      <c r="AJ43" s="16"/>
+      <c r="AK43" s="16"/>
+      <c r="AL43" s="17"/>
       <c r="AM43" s="1"/>
-      <c r="AN43" s="16" t="s">
+      <c r="AN43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AO43" s="17"/>
-      <c r="AP43" s="17"/>
-      <c r="AQ43" s="18"/>
+      <c r="AO43" s="16"/>
+      <c r="AP43" s="16"/>
+      <c r="AQ43" s="17"/>
       <c r="AR43" s="1"/>
-      <c r="AS43" s="16" t="s">
+      <c r="AS43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AT43" s="17"/>
-      <c r="AU43" s="17"/>
-      <c r="AV43" s="18"/>
+      <c r="AT43" s="16"/>
+      <c r="AU43" s="16"/>
+      <c r="AV43" s="17"/>
       <c r="AW43" s="1"/>
-      <c r="AX43" s="16" t="s">
+      <c r="AX43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AY43" s="17"/>
-      <c r="AZ43" s="17"/>
-      <c r="BA43" s="18"/>
+      <c r="AY43" s="16"/>
+      <c r="AZ43" s="16"/>
+      <c r="BA43" s="17"/>
       <c r="BB43" s="1"/>
-      <c r="BC43" s="16" t="s">
+      <c r="BC43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="BD43" s="17"/>
-      <c r="BE43" s="17"/>
-      <c r="BF43" s="18"/>
+      <c r="BD43" s="16"/>
+      <c r="BE43" s="16"/>
+      <c r="BF43" s="17"/>
     </row>
     <row r="44" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AA44" s="6" t="s">
@@ -49147,47 +49147,47 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
-      <c r="AD51" s="16" t="s">
+      <c r="AD51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AE51" s="17"/>
-      <c r="AF51" s="17"/>
-      <c r="AG51" s="18"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
+      <c r="AG51" s="17"/>
       <c r="AH51" s="1"/>
-      <c r="AI51" s="16" t="s">
+      <c r="AI51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
-      <c r="AL51" s="18"/>
+      <c r="AJ51" s="16"/>
+      <c r="AK51" s="16"/>
+      <c r="AL51" s="17"/>
       <c r="AM51" s="1"/>
-      <c r="AN51" s="16" t="s">
+      <c r="AN51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AO51" s="17"/>
-      <c r="AP51" s="17"/>
-      <c r="AQ51" s="18"/>
+      <c r="AO51" s="16"/>
+      <c r="AP51" s="16"/>
+      <c r="AQ51" s="17"/>
       <c r="AR51" s="1"/>
-      <c r="AS51" s="16" t="s">
+      <c r="AS51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AT51" s="17"/>
-      <c r="AU51" s="17"/>
-      <c r="AV51" s="18"/>
+      <c r="AT51" s="16"/>
+      <c r="AU51" s="16"/>
+      <c r="AV51" s="17"/>
       <c r="AW51" s="1"/>
-      <c r="AX51" s="16" t="s">
+      <c r="AX51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AY51" s="17"/>
-      <c r="AZ51" s="17"/>
-      <c r="BA51" s="18"/>
+      <c r="AY51" s="16"/>
+      <c r="AZ51" s="16"/>
+      <c r="BA51" s="17"/>
       <c r="BB51" s="1"/>
-      <c r="BC51" s="16" t="s">
+      <c r="BC51" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="BD51" s="17"/>
-      <c r="BE51" s="17"/>
-      <c r="BF51" s="18"/>
+      <c r="BD51" s="16"/>
+      <c r="BE51" s="16"/>
+      <c r="BF51" s="17"/>
     </row>
     <row r="52" spans="27:58" x14ac:dyDescent="0.3">
       <c r="AA52" s="6" t="s">
@@ -49718,47 +49718,47 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
       <c r="AC59" s="1"/>
-      <c r="AD59" s="16" t="s">
+      <c r="AD59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AE59" s="17"/>
-      <c r="AF59" s="17"/>
-      <c r="AG59" s="18"/>
+      <c r="AE59" s="16"/>
+      <c r="AF59" s="16"/>
+      <c r="AG59" s="17"/>
       <c r="AH59" s="1"/>
-      <c r="AI59" s="16" t="s">
+      <c r="AI59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AJ59" s="17"/>
-      <c r="AK59" s="17"/>
-      <c r="AL59" s="18"/>
+      <c r="AJ59" s="16"/>
+      <c r="AK59" s="16"/>
+      <c r="AL59" s="17"/>
       <c r="AM59" s="1"/>
-      <c r="AN59" s="16" t="s">
+      <c r="AN59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AO59" s="17"/>
-      <c r="AP59" s="17"/>
-      <c r="AQ59" s="18"/>
+      <c r="AO59" s="16"/>
+      <c r="AP59" s="16"/>
+      <c r="AQ59" s="17"/>
       <c r="AR59" s="1"/>
-      <c r="AS59" s="16" t="s">
+      <c r="AS59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AT59" s="17"/>
-      <c r="AU59" s="17"/>
-      <c r="AV59" s="18"/>
+      <c r="AT59" s="16"/>
+      <c r="AU59" s="16"/>
+      <c r="AV59" s="17"/>
       <c r="AW59" s="1"/>
-      <c r="AX59" s="16" t="s">
+      <c r="AX59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AY59" s="17"/>
-      <c r="AZ59" s="17"/>
-      <c r="BA59" s="18"/>
+      <c r="AY59" s="16"/>
+      <c r="AZ59" s="16"/>
+      <c r="BA59" s="17"/>
       <c r="BB59" s="1"/>
-      <c r="BC59" s="16" t="s">
+      <c r="BC59" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="BD59" s="17"/>
-      <c r="BE59" s="17"/>
-      <c r="BF59" s="18"/>
+      <c r="BD59" s="16"/>
+      <c r="BE59" s="16"/>
+      <c r="BF59" s="17"/>
     </row>
     <row r="60" spans="27:58" x14ac:dyDescent="0.3">
       <c r="AA60" s="6" t="s">
@@ -50253,24 +50253,31 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="AD11:AG11"/>
-    <mergeCell ref="AI11:AL11"/>
-    <mergeCell ref="AN11:AQ11"/>
-    <mergeCell ref="AS11:AV11"/>
-    <mergeCell ref="BC1:BF1"/>
-    <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="AI3:AL3"/>
-    <mergeCell ref="AN3:AQ3"/>
-    <mergeCell ref="AS3:AV3"/>
-    <mergeCell ref="AX3:BA3"/>
-    <mergeCell ref="BC3:BF3"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="BC59:BF59"/>
+    <mergeCell ref="AD51:AG51"/>
+    <mergeCell ref="AI51:AL51"/>
+    <mergeCell ref="AN51:AQ51"/>
+    <mergeCell ref="AS51:AV51"/>
+    <mergeCell ref="AX51:BA51"/>
+    <mergeCell ref="BC51:BF51"/>
+    <mergeCell ref="AD59:AG59"/>
+    <mergeCell ref="AI59:AL59"/>
+    <mergeCell ref="AN59:AQ59"/>
+    <mergeCell ref="AS59:AV59"/>
+    <mergeCell ref="AX59:BA59"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="AD35:AG35"/>
+    <mergeCell ref="AI35:AL35"/>
+    <mergeCell ref="AN35:AQ35"/>
+    <mergeCell ref="AS35:AV35"/>
+    <mergeCell ref="BC35:BF35"/>
+    <mergeCell ref="AD43:AG43"/>
+    <mergeCell ref="AI43:AL43"/>
+    <mergeCell ref="AN43:AQ43"/>
+    <mergeCell ref="AS43:AV43"/>
+    <mergeCell ref="AX43:BA43"/>
+    <mergeCell ref="BC43:BF43"/>
+    <mergeCell ref="AX35:BA35"/>
     <mergeCell ref="BC27:BF27"/>
     <mergeCell ref="BC11:BF11"/>
     <mergeCell ref="C19:H19"/>
@@ -50286,31 +50293,24 @@
     <mergeCell ref="AS27:AV27"/>
     <mergeCell ref="AX27:BA27"/>
     <mergeCell ref="AX11:BA11"/>
-    <mergeCell ref="BC35:BF35"/>
-    <mergeCell ref="AD43:AG43"/>
-    <mergeCell ref="AI43:AL43"/>
-    <mergeCell ref="AN43:AQ43"/>
-    <mergeCell ref="AS43:AV43"/>
-    <mergeCell ref="AX43:BA43"/>
-    <mergeCell ref="BC43:BF43"/>
-    <mergeCell ref="AX35:BA35"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="AD35:AG35"/>
-    <mergeCell ref="AI35:AL35"/>
-    <mergeCell ref="AN35:AQ35"/>
-    <mergeCell ref="AS35:AV35"/>
-    <mergeCell ref="BC59:BF59"/>
-    <mergeCell ref="AD51:AG51"/>
-    <mergeCell ref="AI51:AL51"/>
-    <mergeCell ref="AN51:AQ51"/>
-    <mergeCell ref="AS51:AV51"/>
-    <mergeCell ref="AX51:BA51"/>
-    <mergeCell ref="BC51:BF51"/>
-    <mergeCell ref="AD59:AG59"/>
-    <mergeCell ref="AI59:AL59"/>
-    <mergeCell ref="AN59:AQ59"/>
-    <mergeCell ref="AS59:AV59"/>
-    <mergeCell ref="AX59:BA59"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="BC1:BF1"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AI3:AL3"/>
+    <mergeCell ref="AN3:AQ3"/>
+    <mergeCell ref="AS3:AV3"/>
+    <mergeCell ref="AX3:BA3"/>
+    <mergeCell ref="BC3:BF3"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="AD11:AG11"/>
+    <mergeCell ref="AI11:AL11"/>
+    <mergeCell ref="AN11:AQ11"/>
+    <mergeCell ref="AS11:AV11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>